<commit_message>
function in lexical order - hidden player ignored
</commit_message>
<xml_diff>
--- a/examples/node-red-contrib-sonos-plus 40  Commands.xlsx
+++ b/examples/node-red-contrib-sonos-plus 40  Commands.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hekla\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\node-red-contrib-sonos-plus\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DE4337-E751-4FF4-9E71-FD2C88C9F216}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126777CB-0369-4387-9F4B-A92D9C2A6622}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{12C28715-236A-4339-BC9B-A8B167B552A0}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{12C28715-236A-4339-BC9B-A8B167B552A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Universal" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="209">
   <si>
     <t>group.adjust.volume</t>
   </si>
@@ -595,9 +595,6 @@
     <t>full new title</t>
   </si>
   <si>
-    <t>new 'volume</t>
-  </si>
-  <si>
     <t>new volume</t>
   </si>
   <si>
@@ -638,6 +635,33 @@
   </si>
   <si>
     <t>volume 0 … 100</t>
+  </si>
+  <si>
+    <t>player.get.bass</t>
+  </si>
+  <si>
+    <t>bass level</t>
+  </si>
+  <si>
+    <t>number -10 … 10</t>
+  </si>
+  <si>
+    <t>player.get.treble</t>
+  </si>
+  <si>
+    <t>treble level</t>
+  </si>
+  <si>
+    <t>player.set.bass</t>
+  </si>
+  <si>
+    <t>-10 … 10</t>
+  </si>
+  <si>
+    <t>player.set.treble</t>
+  </si>
+  <si>
+    <t>new level</t>
   </si>
 </sst>
 </file>
@@ -1406,7 +1430,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1434,6 +1488,96 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
           <bgColor theme="2"/>
         </patternFill>
       </fill>
@@ -1791,31 +1935,31 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.04296875" customWidth="1"/>
+    <col min="1" max="1" width="28.06640625" customWidth="1"/>
     <col min="2" max="2" width="24" style="20" customWidth="1"/>
     <col min="3" max="3" width="14.86328125" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.31640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.19921875" style="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.1328125" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.76953125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.7265625" customWidth="1"/>
-    <col min="10" max="10" width="19.6796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="76.58984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.73046875" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="76.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="1.5">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="28.9" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A1" s="105" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B1" s="106"/>
       <c r="C1" s="106"/>
@@ -1833,16 +1977,16 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="21.4" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A2" s="69" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B2" s="74" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C2" s="75"/>
       <c r="D2" s="88" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E2" s="89"/>
       <c r="F2" s="89"/>
@@ -1857,9 +2001,9 @@
       </c>
       <c r="L2" s="103"/>
     </row>
-    <row r="3" spans="1:12" ht="16.75" thickBot="1" x14ac:dyDescent="0.95">
+    <row r="3" spans="1:12" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="70" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B3" s="76" t="s">
         <v>66</v>
@@ -1868,7 +2012,7 @@
         <v>95</v>
       </c>
       <c r="D3" s="90" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E3" s="58" t="s">
         <v>59</v>
@@ -1893,7 +2037,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="71" t="s">
         <v>0</v>
       </c>
@@ -1901,13 +2045,13 @@
         <v>163</v>
       </c>
       <c r="C4" s="79" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D4" s="78" t="s">
         <v>57</v>
       </c>
       <c r="E4" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F4" s="63" t="s">
         <v>92</v>
@@ -1929,7 +2073,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="72" t="s">
         <v>1</v>
       </c>
@@ -1943,7 +2087,7 @@
         <v>57</v>
       </c>
       <c r="E5" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F5" s="64" t="s">
         <v>92</v>
@@ -1965,7 +2109,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="72" t="s">
         <v>2</v>
       </c>
@@ -1979,7 +2123,7 @@
         <v>111</v>
       </c>
       <c r="E6" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F6" s="64" t="s">
         <v>92</v>
@@ -1999,7 +2143,7 @@
       <c r="K6" s="39"/>
       <c r="L6" s="72"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="72" t="s">
         <v>3</v>
       </c>
@@ -2013,7 +2157,7 @@
         <v>57</v>
       </c>
       <c r="E7" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F7" s="64" t="s">
         <v>92</v>
@@ -2035,7 +2179,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="72" t="s">
         <v>4</v>
       </c>
@@ -2049,7 +2193,7 @@
         <v>57</v>
       </c>
       <c r="E8" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F8" s="64" t="s">
         <v>92</v>
@@ -2071,7 +2215,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="72" t="s">
         <v>5</v>
       </c>
@@ -2085,7 +2229,7 @@
         <v>57</v>
       </c>
       <c r="E9" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F9" s="64" t="s">
         <v>92</v>
@@ -2107,7 +2251,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="72" t="s">
         <v>6</v>
       </c>
@@ -2121,7 +2265,7 @@
         <v>57</v>
       </c>
       <c r="E10" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F10" s="64" t="s">
         <v>92</v>
@@ -2143,7 +2287,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="72" t="s">
         <v>7</v>
       </c>
@@ -2157,7 +2301,7 @@
         <v>57</v>
       </c>
       <c r="E11" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F11" s="64" t="s">
         <v>92</v>
@@ -2179,7 +2323,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="72" t="s">
         <v>8</v>
       </c>
@@ -2193,7 +2337,7 @@
         <v>57</v>
       </c>
       <c r="E12" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F12" s="64" t="s">
         <v>92</v>
@@ -2215,7 +2359,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="72" t="s">
         <v>9</v>
       </c>
@@ -2229,7 +2373,7 @@
         <v>57</v>
       </c>
       <c r="E13" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F13" s="64" t="s">
         <v>92</v>
@@ -2251,7 +2395,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="72" t="s">
         <v>10</v>
       </c>
@@ -2265,7 +2409,7 @@
         <v>57</v>
       </c>
       <c r="E14" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F14" s="64" t="s">
         <v>92</v>
@@ -2287,7 +2431,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="72" t="s">
         <v>11</v>
       </c>
@@ -2301,7 +2445,7 @@
         <v>57</v>
       </c>
       <c r="E15" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F15" s="64" t="s">
         <v>92</v>
@@ -2323,7 +2467,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="72" t="s">
         <v>12</v>
       </c>
@@ -2337,7 +2481,7 @@
         <v>57</v>
       </c>
       <c r="E16" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F16" s="64" t="s">
         <v>92</v>
@@ -2359,7 +2503,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" s="72" t="s">
         <v>13</v>
       </c>
@@ -2373,13 +2517,13 @@
         <v>57</v>
       </c>
       <c r="E17" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F17" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G17" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H17" s="81" t="s">
         <v>92</v>
@@ -2395,7 +2539,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" s="72" t="s">
         <v>14</v>
       </c>
@@ -2409,16 +2553,16 @@
         <v>57</v>
       </c>
       <c r="E18" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F18" s="64" t="s">
         <v>92</v>
       </c>
       <c r="G18" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H18" s="93" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I18" s="67" t="s">
         <v>85</v>
@@ -2431,7 +2575,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="72" t="s">
         <v>15</v>
       </c>
@@ -2445,13 +2589,13 @@
         <v>158</v>
       </c>
       <c r="E19" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F19" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G19" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H19" s="81" t="s">
         <v>92</v>
@@ -2467,7 +2611,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" s="72" t="s">
         <v>16</v>
       </c>
@@ -2481,13 +2625,13 @@
         <v>57</v>
       </c>
       <c r="E20" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F20" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G20" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H20" s="81" t="s">
         <v>92</v>
@@ -2503,7 +2647,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21" s="72" t="s">
         <v>17</v>
       </c>
@@ -2517,7 +2661,7 @@
         <v>57</v>
       </c>
       <c r="E21" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F21" s="64" t="s">
         <v>92</v>
@@ -2539,7 +2683,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A22" s="72" t="s">
         <v>18</v>
       </c>
@@ -2553,13 +2697,13 @@
         <v>57</v>
       </c>
       <c r="E22" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F22" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G22" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H22" s="81" t="s">
         <v>92</v>
@@ -2575,7 +2719,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23" s="72" t="s">
         <v>19</v>
       </c>
@@ -2589,13 +2733,13 @@
         <v>57</v>
       </c>
       <c r="E23" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F23" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G23" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H23" s="81" t="s">
         <v>92</v>
@@ -2611,7 +2755,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24" s="72" t="s">
         <v>20</v>
       </c>
@@ -2625,13 +2769,13 @@
         <v>57</v>
       </c>
       <c r="E24" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F24" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G24" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H24" s="81" t="s">
         <v>92</v>
@@ -2647,7 +2791,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25" s="72" t="s">
         <v>21</v>
       </c>
@@ -2661,7 +2805,7 @@
         <v>57</v>
       </c>
       <c r="E25" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F25" s="64" t="s">
         <v>92</v>
@@ -2683,7 +2827,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A26" s="72" t="s">
         <v>22</v>
       </c>
@@ -2697,7 +2841,7 @@
         <v>159</v>
       </c>
       <c r="E26" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F26" s="64" t="s">
         <v>92</v>
@@ -2719,7 +2863,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A27" s="72" t="s">
         <v>23</v>
       </c>
@@ -2733,7 +2877,7 @@
         <v>57</v>
       </c>
       <c r="E27" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F27" s="64" t="s">
         <v>92</v>
@@ -2755,7 +2899,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A28" s="72" t="s">
         <v>24</v>
       </c>
@@ -2769,7 +2913,7 @@
         <v>57</v>
       </c>
       <c r="E28" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F28" s="64" t="s">
         <v>92</v>
@@ -2791,7 +2935,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A29" s="72" t="s">
         <v>25</v>
       </c>
@@ -2805,7 +2949,7 @@
         <v>57</v>
       </c>
       <c r="E29" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F29" s="64" t="s">
         <v>92</v>
@@ -2827,7 +2971,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A30" s="72" t="s">
         <v>26</v>
       </c>
@@ -2841,7 +2985,7 @@
         <v>57</v>
       </c>
       <c r="E30" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F30" s="64" t="s">
         <v>92</v>
@@ -2863,7 +3007,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A31" s="72" t="s">
         <v>27</v>
       </c>
@@ -2877,7 +3021,7 @@
         <v>57</v>
       </c>
       <c r="E31" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F31" s="64" t="s">
         <v>92</v>
@@ -2899,7 +3043,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A32" s="72" t="s">
         <v>28</v>
       </c>
@@ -2913,7 +3057,7 @@
         <v>57</v>
       </c>
       <c r="E32" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F32" s="64" t="s">
         <v>92</v>
@@ -2935,7 +3079,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A33" s="72" t="s">
         <v>29</v>
       </c>
@@ -2949,7 +3093,7 @@
         <v>57</v>
       </c>
       <c r="E33" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F33" s="64" t="s">
         <v>92</v>
@@ -2971,7 +3115,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A34" s="72" t="s">
         <v>30</v>
       </c>
@@ -2985,7 +3129,7 @@
         <v>57</v>
       </c>
       <c r="E34" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F34" s="64" t="s">
         <v>92</v>
@@ -3007,7 +3151,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A35" s="72" t="s">
         <v>31</v>
       </c>
@@ -3018,7 +3162,7 @@
         <v>93</v>
       </c>
       <c r="D35" s="94" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E35" s="64" t="s">
         <v>92</v>
@@ -3041,7 +3185,7 @@
       <c r="K35" s="39"/>
       <c r="L35" s="72"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A36" s="72" t="s">
         <v>32</v>
       </c>
@@ -3075,7 +3219,7 @@
       <c r="K36" s="41"/>
       <c r="L36" s="72"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A37" s="72" t="s">
         <v>33</v>
       </c>
@@ -3109,7 +3253,7 @@
       <c r="K37" s="39"/>
       <c r="L37" s="72"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A38" s="72" t="s">
         <v>34</v>
       </c>
@@ -3143,12 +3287,12 @@
       <c r="K38" s="39"/>
       <c r="L38" s="72"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A39" s="72" t="s">
         <v>94</v>
       </c>
       <c r="B39" s="80" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C39" s="83" t="s">
         <v>93</v>
@@ -3177,7 +3321,7 @@
       <c r="K39" s="39"/>
       <c r="L39" s="72"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A40" s="72" t="s">
         <v>35</v>
       </c>
@@ -3191,10 +3335,10 @@
         <v>158</v>
       </c>
       <c r="E40" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F40" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G40" s="64" t="s">
         <v>57</v>
@@ -3211,7 +3355,7 @@
       <c r="K40" s="39"/>
       <c r="L40" s="72"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A41" s="72" t="s">
         <v>36</v>
       </c>
@@ -3219,13 +3363,13 @@
         <v>163</v>
       </c>
       <c r="C41" s="83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D41" s="78" t="s">
         <v>57</v>
       </c>
       <c r="E41" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F41" s="64" t="s">
         <v>92</v>
@@ -3247,9 +3391,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A42" s="72" t="s">
-        <v>37</v>
+        <v>200</v>
       </c>
       <c r="B42" s="80" t="s">
         <v>92</v>
@@ -3261,7 +3405,7 @@
         <v>57</v>
       </c>
       <c r="E42" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F42" s="64" t="s">
         <v>92</v>
@@ -3273,19 +3417,19 @@
         <v>92</v>
       </c>
       <c r="I42" s="67" t="s">
-        <v>104</v>
+        <v>201</v>
       </c>
       <c r="J42" s="101" t="s">
-        <v>103</v>
+        <v>202</v>
       </c>
       <c r="K42" s="39"/>
       <c r="L42" s="72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A43" s="72" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B43" s="80" t="s">
         <v>92</v>
@@ -3297,7 +3441,7 @@
         <v>57</v>
       </c>
       <c r="E43" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F43" s="64" t="s">
         <v>92</v>
@@ -3319,9 +3463,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A44" s="72" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B44" s="80" t="s">
         <v>92</v>
@@ -3333,7 +3477,7 @@
         <v>57</v>
       </c>
       <c r="E44" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F44" s="64" t="s">
         <v>92</v>
@@ -3355,9 +3499,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A45" s="72" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B45" s="80" t="s">
         <v>92</v>
@@ -3369,7 +3513,7 @@
         <v>57</v>
       </c>
       <c r="E45" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F45" s="64" t="s">
         <v>92</v>
@@ -3391,9 +3535,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A46" s="72" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B46" s="80" t="s">
         <v>92</v>
@@ -3405,7 +3549,7 @@
         <v>57</v>
       </c>
       <c r="E46" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F46" s="64" t="s">
         <v>92</v>
@@ -3427,9 +3571,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A47" s="72" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B47" s="80" t="s">
         <v>92</v>
@@ -3441,7 +3585,7 @@
         <v>57</v>
       </c>
       <c r="E47" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F47" s="64" t="s">
         <v>92</v>
@@ -3453,19 +3597,19 @@
         <v>92</v>
       </c>
       <c r="I47" s="67" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J47" s="101" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="K47" s="39"/>
       <c r="L47" s="72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A48" s="72" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B48" s="80" t="s">
         <v>92</v>
@@ -3477,7 +3621,7 @@
         <v>57</v>
       </c>
       <c r="E48" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F48" s="64" t="s">
         <v>92</v>
@@ -3489,19 +3633,19 @@
         <v>92</v>
       </c>
       <c r="I48" s="67" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="J48" s="101" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K48" s="39"/>
       <c r="L48" s="72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A49" s="72" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B49" s="80" t="s">
         <v>92</v>
@@ -3513,7 +3657,7 @@
         <v>57</v>
       </c>
       <c r="E49" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F49" s="64" t="s">
         <v>92</v>
@@ -3525,21 +3669,19 @@
         <v>92</v>
       </c>
       <c r="I49" s="67" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="J49" s="101" t="s">
-        <v>109</v>
-      </c>
-      <c r="K49" s="38" t="s">
-        <v>59</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="K49" s="39"/>
       <c r="L49" s="72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A50" s="72" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B50" s="80" t="s">
         <v>92</v>
@@ -3551,7 +3693,7 @@
         <v>57</v>
       </c>
       <c r="E50" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F50" s="64" t="s">
         <v>92</v>
@@ -3563,19 +3705,21 @@
         <v>92</v>
       </c>
       <c r="I50" s="67" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="J50" s="101" t="s">
-        <v>106</v>
-      </c>
-      <c r="K50" s="39"/>
+        <v>109</v>
+      </c>
+      <c r="K50" s="38" t="s">
+        <v>59</v>
+      </c>
       <c r="L50" s="72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A51" s="72" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B51" s="80" t="s">
         <v>92</v>
@@ -3587,7 +3731,7 @@
         <v>57</v>
       </c>
       <c r="E51" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F51" s="64" t="s">
         <v>92</v>
@@ -3599,102 +3743,106 @@
         <v>92</v>
       </c>
       <c r="I51" s="67" t="s">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="J51" s="101" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K51" s="39"/>
       <c r="L51" s="72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A52" s="72" t="s">
+        <v>203</v>
+      </c>
+      <c r="B52" s="80" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" s="81" t="s">
+        <v>57</v>
+      </c>
+      <c r="D52" s="78" t="s">
+        <v>57</v>
+      </c>
+      <c r="E52" s="62" t="s">
+        <v>187</v>
+      </c>
+      <c r="F52" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="G52" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H52" s="81" t="s">
+        <v>92</v>
+      </c>
+      <c r="I52" s="67" t="s">
+        <v>204</v>
+      </c>
+      <c r="J52" s="101" t="s">
+        <v>202</v>
+      </c>
+      <c r="K52" s="39"/>
+      <c r="L52" s="72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A53" s="72" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53" s="80" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" s="81" t="s">
+        <v>57</v>
+      </c>
+      <c r="D53" s="78" t="s">
+        <v>57</v>
+      </c>
+      <c r="E53" s="62" t="s">
+        <v>187</v>
+      </c>
+      <c r="F53" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="G53" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H53" s="81" t="s">
+        <v>92</v>
+      </c>
+      <c r="I53" s="67" t="s">
+        <v>58</v>
+      </c>
+      <c r="J53" s="101" t="s">
+        <v>107</v>
+      </c>
+      <c r="K53" s="39"/>
+      <c r="L53" s="72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A54" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="B52" s="82" t="s">
+      <c r="B54" s="82" t="s">
         <v>170</v>
       </c>
-      <c r="C52" s="83" t="s">
+      <c r="C54" s="83" t="s">
         <v>93</v>
       </c>
-      <c r="D52" s="78" t="s">
-        <v>57</v>
-      </c>
-      <c r="E52" s="62" t="s">
-        <v>188</v>
-      </c>
-      <c r="F52" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="G52" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H52" s="81" t="s">
-        <v>92</v>
-      </c>
-      <c r="I52" s="67" t="s">
-        <v>85</v>
-      </c>
-      <c r="J52" s="101" t="s">
-        <v>57</v>
-      </c>
-      <c r="K52" s="39"/>
-      <c r="L52" s="72"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.75">
-      <c r="A53" s="72" t="s">
-        <v>48</v>
-      </c>
-      <c r="B53" s="80" t="s">
-        <v>92</v>
-      </c>
-      <c r="C53" s="81" t="s">
-        <v>57</v>
-      </c>
-      <c r="D53" s="78" t="s">
-        <v>57</v>
-      </c>
-      <c r="E53" s="62" t="s">
-        <v>188</v>
-      </c>
-      <c r="F53" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="G53" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H53" s="81" t="s">
-        <v>92</v>
-      </c>
-      <c r="I53" s="67" t="s">
-        <v>85</v>
-      </c>
-      <c r="J53" s="101" t="s">
-        <v>57</v>
-      </c>
-      <c r="K53" s="39"/>
-      <c r="L53" s="72"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.75">
-      <c r="A54" s="72" t="s">
-        <v>49</v>
-      </c>
-      <c r="B54" s="82" t="s">
-        <v>171</v>
-      </c>
-      <c r="C54" s="83" t="s">
-        <v>165</v>
-      </c>
       <c r="D54" s="78" t="s">
         <v>57</v>
       </c>
       <c r="E54" s="62" t="s">
-        <v>188</v>
-      </c>
-      <c r="F54" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
+      </c>
+      <c r="F54" s="64" t="s">
+        <v>92</v>
       </c>
       <c r="G54" s="64" t="s">
         <v>92</v>
@@ -3709,25 +3857,23 @@
         <v>57</v>
       </c>
       <c r="K54" s="39"/>
-      <c r="L54" s="72" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="L54" s="72"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A55" s="72" t="s">
-        <v>50</v>
-      </c>
-      <c r="B55" s="82" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" s="83" t="s">
-        <v>63</v>
+        <v>48</v>
+      </c>
+      <c r="B55" s="80" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" s="81" t="s">
+        <v>57</v>
       </c>
       <c r="D55" s="78" t="s">
         <v>57</v>
       </c>
       <c r="E55" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F55" s="64" t="s">
         <v>92</v>
@@ -3745,28 +3891,26 @@
         <v>57</v>
       </c>
       <c r="K55" s="39"/>
-      <c r="L55" s="72" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="L55" s="72"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A56" s="72" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B56" s="82" t="s">
-        <v>63</v>
+        <v>171</v>
       </c>
       <c r="C56" s="83" t="s">
-        <v>63</v>
+        <v>165</v>
       </c>
       <c r="D56" s="78" t="s">
         <v>57</v>
       </c>
       <c r="E56" s="62" t="s">
-        <v>188</v>
-      </c>
-      <c r="F56" s="64" t="s">
-        <v>92</v>
+        <v>187</v>
+      </c>
+      <c r="F56" s="62" t="s">
+        <v>187</v>
       </c>
       <c r="G56" s="64" t="s">
         <v>92</v>
@@ -3782,24 +3926,24 @@
       </c>
       <c r="K56" s="39"/>
       <c r="L56" s="72" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.75">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A57" s="72" t="s">
-        <v>52</v>
+        <v>205</v>
       </c>
       <c r="B57" s="82" t="s">
-        <v>63</v>
-      </c>
-      <c r="C57" s="83" t="s">
-        <v>63</v>
+        <v>208</v>
+      </c>
+      <c r="C57" s="81" t="s">
+        <v>206</v>
       </c>
       <c r="D57" s="78" t="s">
         <v>57</v>
       </c>
       <c r="E57" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F57" s="64" t="s">
         <v>92</v>
@@ -3821,9 +3965,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A58" s="72" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B58" s="82" t="s">
         <v>63</v>
@@ -3835,7 +3979,7 @@
         <v>57</v>
       </c>
       <c r="E58" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F58" s="64" t="s">
         <v>92</v>
@@ -3857,9 +4001,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A59" s="72" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B59" s="82" t="s">
         <v>63</v>
@@ -3871,7 +4015,7 @@
         <v>57</v>
       </c>
       <c r="E59" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F59" s="64" t="s">
         <v>92</v>
@@ -3893,21 +4037,21 @@
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A60" s="72" t="s">
-        <v>55</v>
-      </c>
-      <c r="B60" s="80" t="s">
-        <v>186</v>
+        <v>52</v>
+      </c>
+      <c r="B60" s="82" t="s">
+        <v>63</v>
       </c>
       <c r="C60" s="83" t="s">
-        <v>172</v>
+        <v>63</v>
       </c>
       <c r="D60" s="78" t="s">
         <v>57</v>
       </c>
       <c r="E60" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F60" s="64" t="s">
         <v>92</v>
@@ -3929,53 +4073,237 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A61" s="73" t="s">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A61" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="C61" s="83" t="s">
+        <v>63</v>
+      </c>
+      <c r="D61" s="78" t="s">
+        <v>57</v>
+      </c>
+      <c r="E61" s="62" t="s">
+        <v>187</v>
+      </c>
+      <c r="F61" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="G61" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H61" s="81" t="s">
+        <v>92</v>
+      </c>
+      <c r="I61" s="67" t="s">
+        <v>85</v>
+      </c>
+      <c r="J61" s="101" t="s">
+        <v>57</v>
+      </c>
+      <c r="K61" s="39"/>
+      <c r="L61" s="72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A62" s="72" t="s">
+        <v>54</v>
+      </c>
+      <c r="B62" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62" s="83" t="s">
+        <v>63</v>
+      </c>
+      <c r="D62" s="78" t="s">
+        <v>57</v>
+      </c>
+      <c r="E62" s="62" t="s">
+        <v>187</v>
+      </c>
+      <c r="F62" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="G62" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H62" s="81" t="s">
+        <v>92</v>
+      </c>
+      <c r="I62" s="67" t="s">
+        <v>85</v>
+      </c>
+      <c r="J62" s="101" t="s">
+        <v>57</v>
+      </c>
+      <c r="K62" s="39"/>
+      <c r="L62" s="72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A63" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="B63" s="80" t="s">
+        <v>186</v>
+      </c>
+      <c r="C63" s="83" t="s">
+        <v>172</v>
+      </c>
+      <c r="D63" s="78" t="s">
+        <v>57</v>
+      </c>
+      <c r="E63" s="62" t="s">
+        <v>187</v>
+      </c>
+      <c r="F63" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="G63" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H63" s="81" t="s">
+        <v>92</v>
+      </c>
+      <c r="I63" s="67" t="s">
+        <v>85</v>
+      </c>
+      <c r="J63" s="101" t="s">
+        <v>57</v>
+      </c>
+      <c r="K63" s="39"/>
+      <c r="L63" s="72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A64" s="72" t="s">
+        <v>207</v>
+      </c>
+      <c r="B64" s="82" t="s">
+        <v>208</v>
+      </c>
+      <c r="C64" s="81" t="s">
+        <v>206</v>
+      </c>
+      <c r="D64" s="78" t="s">
+        <v>57</v>
+      </c>
+      <c r="E64" s="62" t="s">
+        <v>187</v>
+      </c>
+      <c r="F64" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="G64" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H64" s="81" t="s">
+        <v>92</v>
+      </c>
+      <c r="I64" s="67" t="s">
+        <v>85</v>
+      </c>
+      <c r="J64" s="101" t="s">
+        <v>57</v>
+      </c>
+      <c r="K64" s="39"/>
+      <c r="L64" s="72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A65" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="B61" s="86" t="s">
-        <v>187</v>
-      </c>
-      <c r="C61" s="87" t="s">
-        <v>200</v>
-      </c>
-      <c r="D61" s="95" t="s">
-        <v>57</v>
-      </c>
-      <c r="E61" s="96" t="s">
-        <v>188</v>
-      </c>
-      <c r="F61" s="97" t="s">
-        <v>92</v>
-      </c>
-      <c r="G61" s="97" t="s">
-        <v>92</v>
-      </c>
-      <c r="H61" s="98" t="s">
-        <v>92</v>
-      </c>
-      <c r="I61" s="68" t="s">
+      <c r="B65" s="86" t="s">
+        <v>186</v>
+      </c>
+      <c r="C65" s="87" t="s">
+        <v>199</v>
+      </c>
+      <c r="D65" s="95" t="s">
+        <v>57</v>
+      </c>
+      <c r="E65" s="96" t="s">
+        <v>187</v>
+      </c>
+      <c r="F65" s="97" t="s">
+        <v>92</v>
+      </c>
+      <c r="G65" s="97" t="s">
+        <v>92</v>
+      </c>
+      <c r="H65" s="98" t="s">
+        <v>92</v>
+      </c>
+      <c r="I65" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="J61" s="102" t="s">
-        <v>57</v>
-      </c>
-      <c r="K61" s="43"/>
-      <c r="L61" s="73" t="s">
+      <c r="J65" s="102" t="s">
+        <v>57</v>
+      </c>
+      <c r="K65" s="43"/>
+      <c r="L65" s="73" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:L61">
-    <sortCondition ref="A4:A61"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:L65">
+    <sortCondition ref="A4:A65"/>
   </sortState>
-  <conditionalFormatting sqref="E4:H61">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="ignored">
+  <conditionalFormatting sqref="E4:H41 E43:H51 E53:H56 E58:H63 E65:H65">
+    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="ignored">
       <formula>NOT(ISERROR(SEARCH("ignored",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:L61">
-    <cfRule type="expression" dxfId="6" priority="4">
+  <conditionalFormatting sqref="A4:L41 A43:L51 A53:L56 A58:L63 A65:L65">
+    <cfRule type="expression" dxfId="18" priority="16">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42:H42">
+    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="ignored">
+      <formula>NOT(ISERROR(SEARCH("ignored",E42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42:L42">
+    <cfRule type="expression" dxfId="15" priority="10">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E52:H52">
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="ignored">
+      <formula>NOT(ISERROR(SEARCH("ignored",E52)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52:L52">
+    <cfRule type="expression" dxfId="12" priority="7">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57:H57">
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="ignored">
+      <formula>NOT(ISERROR(SEARCH("ignored",E57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57:L57">
+    <cfRule type="expression" dxfId="9" priority="4">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E64:H64">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="ignored">
+      <formula>NOT(ISERROR(SEARCH("ignored",E64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64:L64">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3985,7 +4313,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{1556FE7F-47CC-4BB7-BBF9-3F28C014F253}">
+          <x14:cfRule type="containsText" priority="20" operator="containsText" id="{1556FE7F-47CC-4BB7-BBF9-3F28C014F253}">
             <xm:f>NOT(ISERROR(SEARCH("ignored",B4)))</xm:f>
             <xm:f>"ignored"</xm:f>
             <x14:dxf>
@@ -4001,7 +4329,83 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C4 B5:C61</xm:sqref>
+          <xm:sqref>C4 B5:C41 B43:C51 B53:C56 B58:C63 B65:C65</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{06343100-0CC5-4265-9340-32C52B858DAA}">
+            <xm:f>NOT(ISERROR(SEARCH("ignored",B42)))</xm:f>
+            <xm:f>"ignored"</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+                <color theme="0" tint="-0.34998626667073579"/>
+              </font>
+              <fill>
+                <patternFill patternType="none">
+                  <bgColor auto="1"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>B42:C42</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{F50224FF-908A-4752-B859-31EA26E3A671}">
+            <xm:f>NOT(ISERROR(SEARCH("ignored",B52)))</xm:f>
+            <xm:f>"ignored"</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+                <color theme="0" tint="-0.34998626667073579"/>
+              </font>
+              <fill>
+                <patternFill patternType="none">
+                  <bgColor auto="1"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>B52:C52</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{6E2188D2-4170-4BDA-A538-80F9A47C11A4}">
+            <xm:f>NOT(ISERROR(SEARCH("ignored",B57)))</xm:f>
+            <xm:f>"ignored"</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+                <color theme="0" tint="-0.34998626667073579"/>
+              </font>
+              <fill>
+                <patternFill patternType="none">
+                  <bgColor auto="1"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>B57:C57</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{FA22152F-42A3-41DE-AE96-08EF0D8FDFF8}">
+            <xm:f>NOT(ISERROR(SEARCH("ignored",B64)))</xm:f>
+            <xm:f>"ignored"</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+                <color theme="0" tint="-0.34998626667073579"/>
+              </font>
+              <fill>
+                <patternFill patternType="none">
+                  <bgColor auto="1"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>B64:C64</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4020,25 +4424,25 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.04296875" customWidth="1"/>
-    <col min="2" max="2" width="23.31640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.06640625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.86328125" customWidth="1"/>
     <col min="4" max="4" width="20" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="20" customWidth="1"/>
-    <col min="6" max="6" width="7.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" style="20" customWidth="1"/>
-    <col min="8" max="8" width="10.76953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.76953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.6796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="76.58984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.19921875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.19921875" style="20" customWidth="1"/>
+    <col min="8" max="8" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="76.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="28.75" x14ac:dyDescent="1.35">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.85">
       <c r="A1" s="46" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B1" s="47"/>
       <c r="C1" s="47"/>
@@ -4056,12 +4460,12 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="21.4" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A2" s="50" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C2" s="52"/>
       <c r="D2" s="53" t="s">
@@ -4080,9 +4484,9 @@
       </c>
       <c r="L2" s="30"/>
     </row>
-    <row r="3" spans="1:12" ht="16.75" thickBot="1" x14ac:dyDescent="0.95">
+    <row r="3" spans="1:12" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="54" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B3" s="55" t="s">
         <v>66</v>
@@ -4091,7 +4495,7 @@
         <v>95</v>
       </c>
       <c r="D3" s="57" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E3" s="58" t="s">
         <v>59</v>
@@ -4116,7 +4520,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="35" t="s">
         <v>118</v>
       </c>
@@ -4127,7 +4531,7 @@
         <v>65</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E4" s="32" t="s">
         <v>92</v>
@@ -4152,7 +4556,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="35" t="s">
         <v>117</v>
       </c>
@@ -4188,7 +4592,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="35" t="s">
         <v>116</v>
       </c>
@@ -4224,7 +4628,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="36" t="s">
         <v>114</v>
       </c>
@@ -4260,7 +4664,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="35" t="s">
         <v>115</v>
       </c>
@@ -4271,7 +4675,7 @@
         <v>57</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E8" s="32" t="s">
         <v>92</v>
@@ -4296,7 +4700,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="35" t="s">
         <v>113</v>
       </c>
@@ -4332,7 +4736,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="10" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="37" t="s">
         <v>112</v>
       </c>
@@ -4370,17 +4774,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4:H10">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="ignored">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="ignored">
       <formula>NOT(ISERROR(SEARCH("ignored",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:L10">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B10">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"ignored"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4397,17 +4801,17 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.90625" customWidth="1"/>
-    <col min="5" max="5" width="15.76953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.58984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.9296875" customWidth="1"/>
+    <col min="5" max="5" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="8" t="s">
         <v>136</v>
       </c>
@@ -4427,7 +4831,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>61</v>
       </c>
@@ -4447,7 +4851,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>156</v>
       </c>
@@ -4463,7 +4867,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>63</v>
       </c>
@@ -4481,7 +4885,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>93</v>
       </c>
@@ -4501,7 +4905,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>148</v>
       </c>
@@ -4521,7 +4925,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>175</v>
       </c>
@@ -4539,7 +4943,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>130</v>
       </c>
@@ -4559,7 +4963,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>60</v>
       </c>
@@ -4579,7 +4983,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>119</v>
       </c>
@@ -4597,7 +5001,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>157</v>
       </c>
@@ -4611,7 +5015,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>64</v>
       </c>
@@ -4631,7 +5035,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>65</v>
       </c>
@@ -4651,7 +5055,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>165</v>
       </c>
@@ -4671,7 +5075,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="15" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="10" t="s">
         <v>58</v>
       </c>
@@ -4694,12 +5098,12 @@
     <sortCondition ref="A2:A15"/>
   </sortState>
   <conditionalFormatting sqref="B2:B15">
-    <cfRule type="notContainsText" dxfId="1" priority="2" operator="notContains" text="ignored">
+    <cfRule type="notContainsText" dxfId="4" priority="2" operator="notContains" text="ignored">
       <formula>ISERROR(SEARCH("ignored",B2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F15">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
ESLint 2 spaces indent, LF, single quotes, no semicolon everwhere
</commit_message>
<xml_diff>
--- a/examples/node-red-contrib-sonos-plus 40  Commands.xlsx
+++ b/examples/node-red-contrib-sonos-plus 40  Commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\node-red-contrib-sonos-plus\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C22379E-B495-4A77-BEB0-F496EAE883BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CB2110-3F6B-4120-9ED4-E88A765CFD6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{12C28715-236A-4339-BC9B-A8B167B552A0}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="2" xr2:uid="{12C28715-236A-4339-BC9B-A8B167B552A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Universal" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="243">
   <si>
     <t>group.adjust.volume</t>
   </si>
@@ -746,13 +746,31 @@
   </si>
   <si>
     <t>coordinator.delegate</t>
+  </si>
+  <si>
+    <t>playback states</t>
+  </si>
+  <si>
+    <t>'stopped' 'playing' 'paused' 'transitioning' 'no_media'</t>
+  </si>
+  <si>
+    <t>queue states</t>
+  </si>
+  <si>
+    <t>'NORMAL' 'REPEAT_ONE' 'REPEAT_ALL' 'SHUFFLE' 'SHUFFLE_NOREPEAT' 'SHUFFLE_REPEAT_ONE'</t>
+  </si>
+  <si>
+    <t>'Sonos Beam' 'Sonos Playbar' 'Sonos Playbase' 'Sonos Arc'</t>
+  </si>
+  <si>
+    <t>Player with tv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -826,6 +844,13 @@
       <name val="Wingdings 2"/>
       <family val="1"/>
       <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1311,7 +1336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1514,11 +1539,19 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="43">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1546,74 +1579,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
           <bgColor theme="2"/>
         </patternFill>
       </fill>
@@ -1740,6 +1705,74 @@
       <font>
         <b val="0"/>
         <i val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="0" tint="-0.34998626667073579"/>
       </font>
       <fill>
@@ -2243,8 +2276,8 @@
   </sheetPr>
   <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4924,127 +4957,127 @@
     <sortCondition ref="A5:A75"/>
   </sortState>
   <conditionalFormatting sqref="E5:H7 E53:H61 E63:H66 E68:H73 E75:H75 E31:H33 E10:H28 E35:H41 E43:H51">
-    <cfRule type="containsText" dxfId="41" priority="41" operator="containsText" text="ignored">
+    <cfRule type="containsText" dxfId="42" priority="41" operator="containsText" text="ignored">
       <formula>NOT(ISERROR(SEARCH("ignored",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:L7 A53:L61 A63:L66 A68:L73 A75:L75 A31:L33 A10:L28 A35:L41 A43:L50 B51:L51">
-    <cfRule type="expression" dxfId="40" priority="38">
+    <cfRule type="expression" dxfId="41" priority="38">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52:H52">
-    <cfRule type="containsText" dxfId="39" priority="33" operator="containsText" text="ignored">
+    <cfRule type="containsText" dxfId="40" priority="33" operator="containsText" text="ignored">
       <formula>NOT(ISERROR(SEARCH("ignored",E52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52:L52">
-    <cfRule type="expression" dxfId="38" priority="32">
+    <cfRule type="expression" dxfId="39" priority="32">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62:H62">
-    <cfRule type="containsText" dxfId="37" priority="30" operator="containsText" text="ignored">
+    <cfRule type="containsText" dxfId="38" priority="30" operator="containsText" text="ignored">
       <formula>NOT(ISERROR(SEARCH("ignored",E62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:L62">
-    <cfRule type="expression" dxfId="36" priority="29">
+    <cfRule type="expression" dxfId="37" priority="29">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67:H67">
-    <cfRule type="containsText" dxfId="35" priority="27" operator="containsText" text="ignored">
+    <cfRule type="containsText" dxfId="36" priority="27" operator="containsText" text="ignored">
       <formula>NOT(ISERROR(SEARCH("ignored",E67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67:L67">
-    <cfRule type="expression" dxfId="34" priority="26">
+    <cfRule type="expression" dxfId="35" priority="26">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74:H74">
-    <cfRule type="containsText" dxfId="33" priority="24" operator="containsText" text="ignored">
+    <cfRule type="containsText" dxfId="34" priority="24" operator="containsText" text="ignored">
       <formula>NOT(ISERROR(SEARCH("ignored",E74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A74:L74">
-    <cfRule type="expression" dxfId="32" priority="23">
+    <cfRule type="expression" dxfId="33" priority="23">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:H29">
-    <cfRule type="containsText" dxfId="31" priority="21" operator="containsText" text="ignored">
+    <cfRule type="containsText" dxfId="32" priority="21" operator="containsText" text="ignored">
       <formula>NOT(ISERROR(SEARCH("ignored",E29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:L29">
-    <cfRule type="expression" dxfId="30" priority="20">
+    <cfRule type="expression" dxfId="31" priority="20">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:H30">
-    <cfRule type="containsText" dxfId="29" priority="18" operator="containsText" text="ignored">
+    <cfRule type="containsText" dxfId="30" priority="18" operator="containsText" text="ignored">
       <formula>NOT(ISERROR(SEARCH("ignored",E30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:L30">
-    <cfRule type="expression" dxfId="28" priority="17">
+    <cfRule type="expression" dxfId="29" priority="17">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:H34">
-    <cfRule type="containsText" dxfId="27" priority="15" operator="containsText" text="ignored">
+    <cfRule type="containsText" dxfId="28" priority="15" operator="containsText" text="ignored">
       <formula>NOT(ISERROR(SEARCH("ignored",E34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:L34">
-    <cfRule type="expression" dxfId="26" priority="14">
+    <cfRule type="expression" dxfId="27" priority="14">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:H9">
-    <cfRule type="containsText" dxfId="25" priority="12" operator="containsText" text="ignored">
+    <cfRule type="containsText" dxfId="26" priority="12" operator="containsText" text="ignored">
       <formula>NOT(ISERROR(SEARCH("ignored",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:L9">
-    <cfRule type="expression" dxfId="24" priority="11">
+    <cfRule type="expression" dxfId="25" priority="11">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8:H8">
-    <cfRule type="containsText" dxfId="23" priority="9" operator="containsText" text="ignored">
+    <cfRule type="containsText" dxfId="24" priority="9" operator="containsText" text="ignored">
       <formula>NOT(ISERROR(SEARCH("ignored",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:L8">
-    <cfRule type="expression" dxfId="22" priority="8">
+    <cfRule type="expression" dxfId="23" priority="8">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42:H42">
-    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="ignored">
+    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="ignored">
       <formula>NOT(ISERROR(SEARCH("ignored",E42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:L42">
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="21" priority="5">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:H4">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="ignored">
+    <cfRule type="containsText" dxfId="19" priority="2" operator="containsText" text="ignored">
       <formula>NOT(ISERROR(SEARCH("ignored",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:L4">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5648,17 +5681,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4:H10">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="ignored">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="ignored">
       <formula>NOT(ISERROR(SEARCH("ignored",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:L10">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B10">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"ignored"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5669,10 +5702,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D058AD-C5D7-4A04-87B2-AA9255366B4A}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5984,16 +6017,45 @@
         <v>155</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" s="114" t="s">
+        <v>239</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B19" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B20" t="s">
+        <v>241</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F16">
     <sortCondition ref="A2:A16"/>
   </sortState>
   <conditionalFormatting sqref="B2:B16">
-    <cfRule type="notContainsText" dxfId="1" priority="2" operator="notContains" text="ignored">
+    <cfRule type="notContainsText" dxfId="2" priority="3" operator="notContains" text="ignored">
       <formula>ISERROR(SEARCH("ignored",B2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:F16">
+  <conditionalFormatting sqref="A2:F16 A18">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>